<commit_message>
added funtionality for putting and getting parts from the resource
</commit_message>
<xml_diff>
--- a/customSim/LES/systemDefinition/Process.xlsx
+++ b/customSim/LES/systemDefinition/Process.xlsx
@@ -1,37 +1,126 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\Thesis\Simulation\customSim\LES\systemDefinition\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB530068-136D-4715-A172-E7A97AC9407B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Process" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Process" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+  <si>
+    <t>env</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>proc_time</t>
+  </si>
+  <si>
+    <t>operating_cost</t>
+  </si>
+  <si>
+    <t>operators</t>
+  </si>
+  <si>
+    <t>operating_status</t>
+  </si>
+  <si>
+    <t>upstream_processes</t>
+  </si>
+  <si>
+    <t>downstream_processes</t>
+  </si>
+  <si>
+    <t>sub_processes</t>
+  </si>
+  <si>
+    <t>skills</t>
+  </si>
+  <si>
+    <t>input_products</t>
+  </si>
+  <si>
+    <t>output_products</t>
+  </si>
+  <si>
+    <t>resources</t>
+  </si>
+  <si>
+    <t>kwargs</t>
+  </si>
+  <si>
+    <t>proc_1</t>
+  </si>
+  <si>
+    <t>proc_2</t>
+  </si>
+  <si>
+    <t>proc_3</t>
+  </si>
+  <si>
+    <t>proc_4</t>
+  </si>
+  <si>
+    <t>proc_5</t>
+  </si>
+  <si>
+    <t>proc_6</t>
+  </si>
+  <si>
+    <t>proc_7</t>
+  </si>
+  <si>
+    <t>proc_8</t>
+  </si>
+  <si>
+    <t>proc_9</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +135,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,92 +459,136 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="B1:O1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:P10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>env</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>proc_time</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>operating_cost</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>operators</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>upstream_processes</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>downstream_processes</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>sub_processes</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>skills</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>input_products</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>output_products</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>resources</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>kwargs</t>
-        </is>
+    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
problem importing data from excel
</commit_message>
<xml_diff>
--- a/customSim/LES/systemDefinition/Process.xlsx
+++ b/customSim/LES/systemDefinition/Process.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\Thesis\Simulation\customSim\LES\systemDefinition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB530068-136D-4715-A172-E7A97AC9407B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59990609-8AD4-400E-A218-CCB065AE69B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3915" yWindow="3915" windowWidth="21585" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Process" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="38">
   <si>
     <t>env</t>
   </si>
@@ -92,6 +92,48 @@
   </si>
   <si>
     <t>proc_9</t>
+  </si>
+  <si>
+    <t>proc_10</t>
+  </si>
+  <si>
+    <t>process_1</t>
+  </si>
+  <si>
+    <t>process_2</t>
+  </si>
+  <si>
+    <t>process_3</t>
+  </si>
+  <si>
+    <t>process_4</t>
+  </si>
+  <si>
+    <t>process_5</t>
+  </si>
+  <si>
+    <t>process_6</t>
+  </si>
+  <si>
+    <t>process_7</t>
+  </si>
+  <si>
+    <t>process_8</t>
+  </si>
+  <si>
+    <t>process_9</t>
+  </si>
+  <si>
+    <t>process_10</t>
+  </si>
+  <si>
+    <t>available</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>{}</t>
   </si>
 </sst>
 </file>
@@ -460,13 +502,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:P10"/>
+  <dimension ref="B1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
@@ -516,75 +563,413 @@
       </c>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
       <c r="C2" t="s">
         <v>15</v>
       </c>
       <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2">
         <v>15</v>
       </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
       <c r="C3" t="s">
         <v>16</v>
       </c>
       <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3">
         <v>16</v>
       </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
       <c r="C4" t="s">
         <v>17</v>
       </c>
       <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4">
         <v>17</v>
       </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" t="s">
+        <v>37</v>
+      </c>
+      <c r="N4" t="s">
+        <v>37</v>
+      </c>
+      <c r="O4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
       <c r="C5" t="s">
         <v>18</v>
       </c>
       <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5">
         <v>18</v>
       </c>
+      <c r="G5">
+        <v>7</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" t="s">
+        <v>36</v>
+      </c>
+      <c r="L5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N5" t="s">
+        <v>37</v>
+      </c>
+      <c r="O5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
       <c r="C6" t="s">
         <v>19</v>
       </c>
       <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6">
         <v>19</v>
       </c>
+      <c r="G6">
+        <v>9</v>
+      </c>
+      <c r="H6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N6" t="s">
+        <v>37</v>
+      </c>
+      <c r="O6" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
       <c r="C7" t="s">
         <v>20</v>
       </c>
       <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7">
         <v>20</v>
       </c>
+      <c r="G7">
+        <v>11</v>
+      </c>
+      <c r="H7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" t="s">
+        <v>37</v>
+      </c>
+      <c r="N7" t="s">
+        <v>37</v>
+      </c>
+      <c r="O7" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
       <c r="C8" t="s">
         <v>21</v>
       </c>
       <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8">
         <v>21</v>
       </c>
+      <c r="G8">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L8" t="s">
+        <v>36</v>
+      </c>
+      <c r="M8" t="s">
+        <v>37</v>
+      </c>
+      <c r="N8" t="s">
+        <v>37</v>
+      </c>
+      <c r="O8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
       <c r="C9" t="s">
         <v>22</v>
       </c>
       <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9">
         <v>22</v>
       </c>
+      <c r="G9">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J9" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" t="s">
+        <v>36</v>
+      </c>
+      <c r="L9" t="s">
+        <v>36</v>
+      </c>
+      <c r="M9" t="s">
+        <v>37</v>
+      </c>
+      <c r="N9" t="s">
+        <v>37</v>
+      </c>
+      <c r="O9" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
       <c r="C10" t="s">
         <v>23</v>
       </c>
       <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10">
         <v>23</v>
+      </c>
+      <c r="G10">
+        <v>17</v>
+      </c>
+      <c r="H10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" t="s">
+        <v>36</v>
+      </c>
+      <c r="L10" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" t="s">
+        <v>37</v>
+      </c>
+      <c r="O10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11">
+        <v>24</v>
+      </c>
+      <c r="G11">
+        <v>19</v>
+      </c>
+      <c r="H11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" t="s">
+        <v>36</v>
+      </c>
+      <c r="J11" t="s">
+        <v>36</v>
+      </c>
+      <c r="K11" t="s">
+        <v>36</v>
+      </c>
+      <c r="L11" t="s">
+        <v>36</v>
+      </c>
+      <c r="M11" t="s">
+        <v>37</v>
+      </c>
+      <c r="N11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O11" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
process mapping is done through excel on;y
</commit_message>
<xml_diff>
--- a/customSim/LES/systemDefinition/Process.xlsx
+++ b/customSim/LES/systemDefinition/Process.xlsx
@@ -17,13 +17,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -42,12 +47,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -75,12 +95,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -451,7 +474,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -581,7 +604,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>['process_6', 'process_7', 'process_8', 'process_9']</t>
+          <t>['process_6', 'process_7', 'process_8', 'process_9', 'processs_10']</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -1290,79 +1313,79 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>env</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>env</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>proc_time</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>operating_cost</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>operators</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>operating_status</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>upstream_processes</t>
         </is>
       </c>
-      <c r="J1" s="2" t="inlineStr">
+      <c r="J1" s="3" t="inlineStr">
         <is>
           <t>downstream_processes</t>
         </is>
       </c>
-      <c r="K1" s="2" t="inlineStr">
+      <c r="K1" s="3" t="inlineStr">
         <is>
           <t>sub_processes</t>
         </is>
       </c>
-      <c r="L1" s="2" t="inlineStr">
+      <c r="L1" s="3" t="inlineStr">
         <is>
           <t>skills</t>
         </is>
       </c>
-      <c r="M1" s="2" t="inlineStr">
+      <c r="M1" s="3" t="inlineStr">
         <is>
           <t>input_products</t>
         </is>
       </c>
-      <c r="N1" s="2" t="inlineStr">
+      <c r="N1" s="3" t="inlineStr">
         <is>
           <t>output_products</t>
         </is>
       </c>
-      <c r="O1" s="2" t="inlineStr">
+      <c r="O1" s="3" t="inlineStr">
         <is>
           <t>resources</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="3" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -1401,7 +1424,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>['process_6', 'process_7', 'process_8', 'process_9']</t>
+          <t>['process_6', 'process_7', 'process_8', 'process_9', 'processs_10']</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -1431,7 +1454,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="3" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -1500,7 +1523,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="3" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
@@ -1569,7 +1592,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n">
+      <c r="A5" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
@@ -1638,7 +1661,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="n">
+      <c r="A6" s="3" t="n">
         <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
@@ -1707,7 +1730,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="n">
+      <c r="A7" s="3" t="n">
         <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
@@ -1776,7 +1799,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="n">
+      <c r="A8" s="3" t="n">
         <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
@@ -1845,7 +1868,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="n">
+      <c r="A9" s="3" t="n">
         <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
@@ -1914,7 +1937,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="n">
+      <c r="A10" s="3" t="n">
         <v>8</v>
       </c>
       <c r="B10" t="inlineStr">
@@ -1983,7 +2006,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="n">
+      <c r="A11" s="3" t="n">
         <v>9</v>
       </c>
       <c r="B11" t="inlineStr">
@@ -2052,7 +2075,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="n">
+      <c r="A12" s="3" t="n">
         <v>10</v>
       </c>
       <c r="B12" t="inlineStr">

</xml_diff>